<commit_message>
richards: completed testing of residual of borehole. no doco yet
r23858
</commit_message>
<xml_diff>
--- a/modules/combined/doc/richards/tests/data/bh.xlsx
+++ b/modules/combined/doc/richards/tests/data/bh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584" firstSheet="12" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="bh02_flow_rate" sheetId="4" r:id="rId1"/>
@@ -23,12 +23,16 @@
     <sheet name="bh05_mass_balance" sheetId="17" r:id="rId14"/>
     <sheet name="bh05" sheetId="14" r:id="rId15"/>
     <sheet name="bh05_expected" sheetId="15" r:id="rId16"/>
+    <sheet name="bh07_steadystate" sheetId="23" r:id="rId17"/>
+    <sheet name="bh07" sheetId="21" r:id="rId18"/>
+    <sheet name="bh07_expected" sheetId="22" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="bh02_" localSheetId="2">'bh02'!$C$3:$H$54</definedName>
     <definedName name="bh02_" localSheetId="6">'bh03'!$C$3:$H$54</definedName>
     <definedName name="bh02_" localSheetId="10">'bh04'!$C$3:$H$24</definedName>
     <definedName name="bh02_" localSheetId="14">'bh05'!$C$3:$H$24</definedName>
+    <definedName name="bh07_" localSheetId="17">'bh07'!$C$3:$J$34</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -84,11 +88,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="5" name="bh07" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\elk\doc\richards\tests\data\bh07.csv" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
   <si>
     <t>time</t>
   </si>
@@ -160,6 +175,54 @@
   </si>
   <si>
     <t>bottomhole</t>
+  </si>
+  <si>
+    <t>P_bh</t>
+  </si>
+  <si>
+    <t>P_R</t>
+  </si>
+  <si>
+    <t>rho_bh</t>
+  </si>
+  <si>
+    <t>rho_R</t>
+  </si>
+  <si>
+    <t>r_bh</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rho</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Seff1VG_Aux</t>
+  </si>
+  <si>
+    <t>ObjectId</t>
+  </si>
+  <si>
+    <t>vtkValidPointMask</t>
+  </si>
+  <si>
+    <t>arc_length</t>
+  </si>
+  <si>
+    <t>Points:0</t>
+  </si>
+  <si>
+    <t>Points:1</t>
+  </si>
+  <si>
+    <t>Points:2</t>
+  </si>
+  <si>
+    <t>1.#QNB</t>
   </si>
 </sst>
 </file>
@@ -23671,6 +23734,652 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Steadystate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-AU" baseline="0"/>
+              <a:t> porepressure distribution due to production borehole</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-AU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>expected</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>bh07_expected!$C$12:$C$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>bh07_expected!$E$12:$E$59</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="48"/>
+                <c:pt idx="0">
+                  <c:v>-4051153.4802910741</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1217913.5301262841</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1930003.6146036</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2435085.8549086973</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2826770.2552887816</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3146742.7801281768</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3417235.7630864112</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3651517.8759723222</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4042964.1433664234</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4362742.1685889103</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4633070.7529928926</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4867210.4932994237</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5073713.6311150817</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5258418.9170882283</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5649550.833826025</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5969072.1071444629</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6239183.6749218907</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6473135.4742678124</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6679472.8729128372</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6864029.9291313533</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7183357.2508779885</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7453304.8832616787</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7687114.7110852264</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7893326.9095293628</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8077771.9922322417</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8244608.2127905702</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8396905.5977245048</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8536995.3704076521</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8666689.4935842268</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8787424.2745137606</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8900357.5220891554</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9006436.1933427565</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9106444.6721767597</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>9201039.9755243044</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9290777.9171536155</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9376132.8803558871</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9457512.9859451801</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9535271.8852979038</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9609718.0412804987</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>9681122.1130502447</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>9749722.8913786113</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>9815732.1130496599</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>9879338.399124369</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>9940710.5017121769</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9999999.9999997932</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10057343.553981729</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10112864.800201757</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>moose</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'bh07'!$I$4:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'bh07'!$C$4:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>212180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4261100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5320600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6029500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6530100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6909800</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7225100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7498300</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7737300</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7937300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8121900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8290200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8437300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8578300</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8703300</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8823600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8932700</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9038700</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9134200</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9229700</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9314300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9398300</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9477800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9551800</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9625700</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9695100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9760900</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9825200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9884500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9942500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="188150912"/>
+        <c:axId val="188152448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="188150912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="300"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>radius (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188152448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="188152448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10000000"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Porepressure</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> (Pa)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188150912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
@@ -23749,6 +24458,17 @@
 </file>
 
 <file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
@@ -23975,6 +24695,33 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9279308" cy="6053271"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bh02" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -23989,6 +24736,10 @@
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bh02" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bh07" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25537,6 +26288,770 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C2:G59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="11.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:7">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="3:7">
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1">
+        <f>$D$2*EXP(D5/$D$3)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7">
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1">
+        <f>$D$2*EXP(D6/$D$3)</f>
+        <v>1005.012520859401</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7">
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7">
+      <c r="C12">
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="1">
+        <f>$G$5+($G$6-$G$5)*LN(C12/$D$8)/LN($D$9/$D$8)</f>
+        <v>997.97647335597696</v>
+      </c>
+      <c r="E12" s="1">
+        <f>$D$3*LN(D12/$D$2)</f>
+        <v>-4051153.4802910741</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f>$G$5+($G$6-$G$5)*LN(C13/$D$8)/LN($D$9/$D$8)</f>
+        <v>1000</v>
+      </c>
+      <c r="E13" s="1">
+        <f>$D$3*LN(D13/$D$2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7">
+      <c r="C14">
+        <f>C13+1</f>
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:D59" si="0">$G$5+($G$6-$G$5)*LN(C14/$D$8)/LN($D$9/$D$8)</f>
+        <v>1000.6091422168762</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" ref="E14:E59" si="1">$D$3*LN(D14/$D$2)</f>
+        <v>1217913.5301262841</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15">
+        <f t="shared" ref="C15:C20" si="2">C14+1</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>1000.9654675713549</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>1930003.6146036</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7">
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>1001.2182844337524</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>2435085.8549086973</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>1001.4143844271468</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>2826770.2552887816</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>1001.5746097882311</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>3146742.7801281768</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5">
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>1001.7100784007805</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>3417235.7630864112</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>1001.8274266506286</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>3651517.8759723222</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
+      <c r="C21">
+        <f>C20+2</f>
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.023526644023</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>4042964.1433664234</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="C22">
+        <f t="shared" ref="C22:C26" si="3">C21+2</f>
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.1837520051073</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>4362742.1685889103</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
+      <c r="C23">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.3192206176567</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>4633070.7529928926</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5">
+      <c r="C24">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.4365688675048</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>4867210.4932994237</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
+      <c r="C25">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.5400773595861</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>5073713.6311150817</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5">
+      <c r="C26">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.6326688608992</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>5258418.9170882283</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
+      <c r="C27">
+        <f>C26+5</f>
+        <v>25</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.8287688542937</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>5649550.833826025</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5">
+      <c r="C28">
+        <f t="shared" ref="C28:C32" si="4">C27+5</f>
+        <v>30</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>1002.9889942153779</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>5969072.1071444629</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5">
+      <c r="C29">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.1244628279273</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>6239183.6749218907</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5">
+      <c r="C30">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.2418110777754</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="1"/>
+        <v>6473135.4742678124</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5">
+      <c r="C31">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.3453195698567</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
+        <v>6679472.8729128372</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5">
+      <c r="C32">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.4379110711699</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="1"/>
+        <v>6864029.9291313533</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5">
+      <c r="C33">
+        <f t="shared" ref="C33:C66" si="5">C32+10</f>
+        <v>60</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.5981364322541</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="1"/>
+        <v>7183357.2508779885</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5">
+      <c r="C34">
+        <f t="shared" si="5"/>
+        <v>70</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.7336050448035</v>
+      </c>
+      <c r="E34" s="1">
+        <f t="shared" si="1"/>
+        <v>7453304.8832616787</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5">
+      <c r="C35">
+        <f t="shared" si="5"/>
+        <v>80</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.8509532946516</v>
+      </c>
+      <c r="E35" s="1">
+        <f t="shared" si="1"/>
+        <v>7687114.7110852264</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5">
+      <c r="C36">
+        <f t="shared" si="5"/>
+        <v>90</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>1003.9544617867328</v>
+      </c>
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>7893326.9095293628</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5">
+      <c r="C37">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.0470532880461</v>
+      </c>
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>8077771.9922322417</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5">
+      <c r="C38">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.1308124893313</v>
+      </c>
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>8244608.2127905702</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5">
+      <c r="C39">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.2072786491303</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>8396905.5977245048</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5">
+      <c r="C40">
+        <f t="shared" si="5"/>
+        <v>130</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.2776206973482</v>
+      </c>
+      <c r="E40" s="1">
+        <f t="shared" si="1"/>
+        <v>8536995.3704076521</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5">
+      <c r="C41">
+        <f t="shared" si="5"/>
+        <v>140</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.3427472616797</v>
+      </c>
+      <c r="E41" s="1">
+        <f t="shared" si="1"/>
+        <v>8666689.4935842268</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5">
+      <c r="C42">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.4033786425248</v>
+      </c>
+      <c r="E42" s="1">
+        <f t="shared" si="1"/>
+        <v>8787424.2745137606</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5">
+      <c r="C43">
+        <f t="shared" si="5"/>
+        <v>160</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.4600955115278</v>
+      </c>
+      <c r="E43" s="1">
+        <f t="shared" si="1"/>
+        <v>8900357.5220891554</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5">
+      <c r="C44">
+        <f t="shared" si="5"/>
+        <v>170</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.5133728205413</v>
+      </c>
+      <c r="E44" s="1">
+        <f t="shared" si="1"/>
+        <v>9006436.1933427565</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5">
+      <c r="C45">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.563604003609</v>
+      </c>
+      <c r="E45" s="1">
+        <f t="shared" si="1"/>
+        <v>9106444.6721767597</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5">
+      <c r="C46">
+        <f t="shared" si="5"/>
+        <v>190</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.6111186266915</v>
+      </c>
+      <c r="E46" s="1">
+        <f t="shared" si="1"/>
+        <v>9201039.9755243044</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5">
+      <c r="C47">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.6561955049223</v>
+      </c>
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>9290777.9171536155</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5">
+      <c r="C48">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.6990726161584</v>
+      </c>
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>9376132.8803558871</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5">
+      <c r="C49">
+        <f t="shared" si="5"/>
+        <v>220</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.7399547062075</v>
+      </c>
+      <c r="E49" s="1">
+        <f t="shared" si="1"/>
+        <v>9457512.9859451801</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5">
+      <c r="C50">
+        <f t="shared" si="5"/>
+        <v>230</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.7790192021124</v>
+      </c>
+      <c r="E50" s="1">
+        <f t="shared" si="1"/>
+        <v>9535271.8852979038</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5">
+      <c r="C51">
+        <f t="shared" si="5"/>
+        <v>240</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.8164208660065</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="1"/>
+        <v>9609718.0412804987</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5">
+      <c r="C52">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="D52" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.8522954983167</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="1"/>
+        <v>9681122.1130502447</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5">
+      <c r="C53">
+        <f t="shared" si="5"/>
+        <v>260</v>
+      </c>
+      <c r="D53" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.8867629142244</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="1"/>
+        <v>9749722.8913786113</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5">
+      <c r="C54">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="D54" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.9199293580879</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="1"/>
+        <v>9815732.1130496599</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5">
+      <c r="C55">
+        <f t="shared" si="5"/>
+        <v>280</v>
+      </c>
+      <c r="D55" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.9518894785559</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="1"/>
+        <v>9879338.399124369</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5">
+      <c r="C56">
+        <f t="shared" si="5"/>
+        <v>290</v>
+      </c>
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>1004.9827279569375</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="1"/>
+        <v>9940710.5017121769</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5">
+      <c r="C57">
+        <f t="shared" si="5"/>
+        <v>300</v>
+      </c>
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>1005.012520859401</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="1"/>
+        <v>9999999.9999997932</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5">
+      <c r="C58">
+        <f t="shared" si="5"/>
+        <v>310</v>
+      </c>
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>1005.0413367673719</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="1"/>
+        <v>10057343.553981729</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5">
+      <c r="C59">
+        <f t="shared" si="5"/>
+        <v>320</v>
+      </c>
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>1005.069237728404</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="1"/>
+        <v>10112864.800201757</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C2:F25"/>
@@ -70750,4 +72265,860 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:J34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10">
+      <c r="C4" s="1">
+        <v>212180</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5" s="1">
+        <v>4261100</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
+        <v>-0.93332999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6" s="1">
+        <v>5320600</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>20</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>20</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-0.86667000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7" s="1">
+        <v>6029500</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>30.001000000000001</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>30</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="C8" s="1">
+        <v>6530100</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>40.000999999999998</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>40</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-0.73333000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="C9" s="1">
+        <v>6909800</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>50.000999999999998</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>50</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-0.66666999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="C10" s="1">
+        <v>7225100</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>60.000999999999998</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>60</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
+      <c r="C11" s="1">
+        <v>7498300</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>70.001999999999995</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-0.53332999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10">
+      <c r="C12" s="1">
+        <v>7737300</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>80.001999999999995</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>80</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-0.46666999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
+      <c r="C13" s="1">
+        <v>7937300</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>90.001999999999995</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>90</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10">
+      <c r="C14" s="1">
+        <v>8121900</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>100</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-0.33333000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
+      <c r="C15" s="1">
+        <v>8290200</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>110</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>110</v>
+      </c>
+      <c r="J15" s="1">
+        <v>-0.26667000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="C16" s="1">
+        <v>8437300</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>120</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>120</v>
+      </c>
+      <c r="J16" s="1">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="C17" s="1">
+        <v>8578300</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>130</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>130</v>
+      </c>
+      <c r="J17" s="1">
+        <v>-0.13333</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10">
+      <c r="C18" s="1">
+        <v>8703300</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>140</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>140</v>
+      </c>
+      <c r="J18" s="1">
+        <v>-6.6667000000000004E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10">
+      <c r="C19" s="1">
+        <v>8823600</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>150</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>150</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10">
+      <c r="C20" s="1">
+        <v>8932700</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>160</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>160</v>
+      </c>
+      <c r="J20" s="1">
+        <v>6.6667000000000004E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10">
+      <c r="C21" s="1">
+        <v>9038700</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>170</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>170</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.13333</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10">
+      <c r="C22" s="1">
+        <v>9134200</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>180</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>180</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10">
+      <c r="C23" s="1">
+        <v>9229700</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1">
+        <v>190</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>190</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.26667000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10">
+      <c r="C24" s="1">
+        <v>9314300</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>200</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>200</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.33333000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10">
+      <c r="C25" s="1">
+        <v>9398300</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>210</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>210</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10">
+      <c r="C26" s="1">
+        <v>9477800</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>220</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>220</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.46666999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10">
+      <c r="C27" s="1">
+        <v>9551800</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>230.01</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>230</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.53332999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10">
+      <c r="C28" s="1">
+        <v>9625700</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>240.01</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>240</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10">
+      <c r="C29" s="1">
+        <v>9695100</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <v>250.01</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>250</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.66666999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10">
+      <c r="C30" s="1">
+        <v>9760900</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>260.01</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>260</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.73333000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10">
+      <c r="C31" s="1">
+        <v>9825200</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>270.01</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>270</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10">
+      <c r="C32" s="1">
+        <v>9884500</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1">
+        <v>280.01</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>280</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.86667000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10">
+      <c r="C33" s="1">
+        <v>9942500</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>290.01</v>
+      </c>
+      <c r="H33" s="1">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <v>290</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.93332999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10">
+      <c r="C34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>300.01</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>300</v>
+      </c>
+      <c r="J34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
richards: doco for tests of boreholes
r23904
</commit_message>
<xml_diff>
--- a/modules/combined/doc/richards/tests/data/bh.xlsx
+++ b/modules/combined/doc/richards/tests/data/bh.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584" firstSheet="12" activeTab="12"/>
+    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584"/>
   </bookViews>
   <sheets>
     <sheet name="bh02_flow_rate" sheetId="4" r:id="rId1"/>
@@ -740,11 +740,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="52923776"/>
-        <c:axId val="52941952"/>
+        <c:axId val="101803136"/>
+        <c:axId val="101804672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52923776"/>
+        <c:axId val="101803136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -770,12 +770,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52941952"/>
+        <c:crossAx val="101804672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52941952"/>
+        <c:axId val="101804672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -806,7 +806,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52923776"/>
+        <c:crossAx val="101803136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1173,11 +1173,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="175116288"/>
-        <c:axId val="175117824"/>
+        <c:axId val="101833728"/>
+        <c:axId val="102110336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="175116288"/>
+        <c:axId val="101833728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -1203,16 +1203,16 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175117824"/>
-        <c:crossesAt val="1.000000000000001E-17"/>
+        <c:crossAx val="102110336"/>
+        <c:crossesAt val="1.0000000000000021E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175117824"/>
+        <c:axId val="102110336"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000008E-14"/>
+          <c:max val="1.0000000000000017E-14"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -1241,7 +1241,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175116288"/>
+        <c:crossAx val="101833728"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1721,11 +1721,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="130999808"/>
-        <c:axId val="174284800"/>
+        <c:axId val="110037248"/>
+        <c:axId val="110051712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130999808"/>
+        <c:axId val="110037248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -1751,12 +1751,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174284800"/>
+        <c:crossAx val="110051712"/>
         <c:crossesAt val="-50"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174284800"/>
+        <c:axId val="110051712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,7 +1787,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130999808"/>
+        <c:crossAx val="110037248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2154,11 +2154,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="179337088"/>
-        <c:axId val="173286528"/>
+        <c:axId val="110265088"/>
+        <c:axId val="110267008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179337088"/>
+        <c:axId val="110265088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -2184,16 +2184,16 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173286528"/>
-        <c:crossesAt val="1.0000000000000021E-17"/>
+        <c:crossAx val="110267008"/>
+        <c:crossesAt val="1.000000000000003E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="173286528"/>
+        <c:axId val="110267008"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000017E-14"/>
+          <c:max val="1.0000000000000025E-14"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -2222,7 +2222,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="179337088"/>
+        <c:crossAx val="110265088"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12647,11 +12647,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="176127360"/>
-        <c:axId val="176178304"/>
+        <c:axId val="110304640"/>
+        <c:axId val="110331392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176127360"/>
+        <c:axId val="110304640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -12677,12 +12677,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176178304"/>
+        <c:crossAx val="110331392"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="176178304"/>
+        <c:axId val="110331392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12713,7 +12713,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176127360"/>
+        <c:crossAx val="110304640"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12900,11 +12900,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="186481664"/>
-        <c:axId val="196134784"/>
+        <c:axId val="110589824"/>
+        <c:axId val="110608384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="186481664"/>
+        <c:axId val="110589824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -12930,16 +12930,16 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196134784"/>
-        <c:crossesAt val="1.0000000000000021E-17"/>
+        <c:crossAx val="110608384"/>
+        <c:crossesAt val="1.000000000000003E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="196134784"/>
+        <c:axId val="110608384"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000006E-12"/>
+          <c:max val="1.0000000000000014E-12"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -12968,7 +12968,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186481664"/>
+        <c:crossAx val="110589824"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23393,11 +23393,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="188947456"/>
-        <c:axId val="188646528"/>
+        <c:axId val="111125632"/>
+        <c:axId val="111127552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188947456"/>
+        <c:axId val="111125632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -23423,12 +23423,12 @@
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188646528"/>
+        <c:crossAx val="111127552"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188646528"/>
+        <c:axId val="111127552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23459,7 +23459,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188947456"/>
+        <c:crossAx val="111125632"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23493,7 +23493,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -23501,10 +23500,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11329691826157727"/>
-          <c:y val="0.1428293892673895"/>
-          <c:w val="0.85614142778750313"/>
-          <c:h val="0.81467127442336551"/>
+          <c:x val="0.11329691826157728"/>
+          <c:y val="0.14282938926738953"/>
+          <c:w val="0.85614142778750324"/>
+          <c:h val="0.81467127442336573"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -23656,11 +23655,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="188645760"/>
-        <c:axId val="186896768"/>
+        <c:axId val="110755200"/>
+        <c:axId val="111166976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188645760"/>
+        <c:axId val="110755200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="-200000"/>
@@ -23682,20 +23681,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186896768"/>
-        <c:crossesAt val="1.000000000000003E-17"/>
+        <c:crossAx val="111166976"/>
+        <c:crossesAt val="1.0000000000000041E-17"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="186896768"/>
+        <c:axId val="111166976"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="1.0000000000000006E-10"/>
+          <c:max val="1.0000000000000012E-10"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
@@ -23720,11 +23718,10 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188645760"/>
+        <c:crossAx val="110755200"/>
         <c:crossesAt val="-200000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23759,7 +23756,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -24298,11 +24294,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="188150912"/>
-        <c:axId val="188152448"/>
+        <c:axId val="111705472"/>
+        <c:axId val="111719936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188150912"/>
+        <c:axId val="111705472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -24324,16 +24320,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188152448"/>
+        <c:crossAx val="111719936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188152448"/>
+        <c:axId val="111719936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000000"/>
@@ -24362,18 +24357,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0E+00" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188150912"/>
+        <c:crossAx val="111705472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -24384,7 +24377,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24395,7 +24388,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24406,7 +24399,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24417,7 +24410,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24428,7 +24421,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24439,7 +24432,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -24450,7 +24443,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="101" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -26671,7 +26664,7 @@
     </row>
     <row r="33" spans="3:5">
       <c r="C33">
-        <f t="shared" ref="C33:C66" si="5">C32+10</f>
+        <f t="shared" ref="C33:C59" si="5">C32+10</f>
         <v>60</v>
       </c>
       <c r="D33" s="1">
@@ -27152,13 +27145,13 @@
         <v>1000000</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:D25" si="0">$D$8*$D$10/$D$11*C15</f>
+        <f t="shared" ref="D15:D24" si="0">$D$8*$D$10/$D$11*C15</f>
         <v>4.5656279846757233</v>
       </c>
     </row>
     <row r="16" spans="3:6">
       <c r="C16">
-        <f t="shared" ref="C16:C25" si="1">C15+1000000</f>
+        <f t="shared" ref="C16:C24" si="1">C15+1000000</f>
         <v>2000000</v>
       </c>
       <c r="D16" s="1">
@@ -28626,7 +28619,7 @@
     </row>
     <row r="16" spans="3:4">
       <c r="C16">
-        <f t="shared" ref="C16:C25" si="1">C15+1000000</f>
+        <f t="shared" ref="C16:C24" si="1">C15+1000000</f>
         <v>2000000</v>
       </c>
       <c r="D16" s="1">
@@ -48955,11 +48948,11 @@
         <v>-3000</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" ref="D15:D34" si="0">$D$8*H15*G15/$D$11*(C15-$G$10)</f>
+        <f t="shared" ref="D15" si="0">$D$8*H15*G15/$D$11*(C15-$G$10)</f>
         <v>4.5519242728301608</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F34" si="1">(1+(-$G$2*C15)^(1/(1-$G$3)))^(-$G$3)</f>
+        <f t="shared" ref="F15" si="1">(1+(-$G$2*C15)^(1/(1-$G$3)))^(-$G$3)</f>
         <v>0.99999998056000028</v>
       </c>
       <c r="G15">
@@ -48967,7 +48960,7 @@
         <v>0.99999999999999889</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" ref="H15:H34" si="3">$G$8*EXP(C15/$G$7)</f>
+        <f t="shared" ref="H15" si="3">$G$8*EXP(C15/$G$7)</f>
         <v>999.99850000112497</v>
       </c>
     </row>
@@ -72140,7 +72133,7 @@
         <v>-1.1539721541502183E-2</v>
       </c>
       <c r="F79">
-        <f t="shared" ref="F79:F142" si="6">(1+(-$G$2*C79)^(1/(1-$G$3)))^(-$G$3)</f>
+        <f t="shared" ref="F79:F84" si="6">(1+(-$G$2*C79)^(1/(1-$G$3)))^(-$G$3)</f>
         <v>6.7259320625271804E-2</v>
       </c>
       <c r="G79">
@@ -72148,7 +72141,7 @@
         <v>1.2962911022952052E-2</v>
       </c>
       <c r="H79" s="1">
-        <f t="shared" ref="H79:H142" si="8">$G$8*EXP(C79/$G$7)</f>
+        <f t="shared" ref="H79:H84" si="8">$G$8*EXP(C79/$G$7)</f>
         <v>999.90250475297046</v>
       </c>
     </row>

</xml_diff>